<commit_message>
Updated the test data file for multiple gateway. generateRandomNumber method,Bug fixes in single gatewaymodule,testdata file for clientdetails
</commit_message>
<xml_diff>
--- a/zf-automation/zf-web/src/main/resources/testdata/MultipleGatewaySpreadsheets/Bulk_Provisioning_GatewayDetails_Existing.xlsx
+++ b/zf-automation/zf-web/src/main/resources/testdata/MultipleGatewaySpreadsheets/Bulk_Provisioning_GatewayDetails_Existing.xlsx
@@ -39,9 +39,6 @@
     <t>Model</t>
   </si>
   <si>
-    <t>MAC_ID</t>
-  </si>
-  <si>
     <t>SERIAL_NO</t>
   </si>
   <si>
@@ -115,6 +112,9 @@
   </si>
   <si>
     <t>12:34:53:81:98</t>
+  </si>
+  <si>
+    <t>MAC_ID/IMEI</t>
   </si>
 </sst>
 </file>
@@ -482,7 +482,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -524,7 +524,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -541,7 +541,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -552,7 +552,7 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -587,63 +587,63 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" t="s">
         <v>30</v>
-      </c>
-      <c r="B2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="J2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="L2" t="s">
-        <v>26</v>
-      </c>
-      <c r="M2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -710,41 +710,41 @@
     </row>
     <row r="8" spans="8:13">
       <c r="L8" t="s">
+        <v>12</v>
+      </c>
+      <c r="M8" t="s">
         <v>13</v>
-      </c>
-      <c r="M8" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="9" spans="8:13">
       <c r="L9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="8:13">
       <c r="L10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="8:13">
       <c r="M11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="8:13">
       <c r="M12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="8:13">
       <c r="M13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>